<commit_message>
CSV fil upload was integrated
</commit_message>
<xml_diff>
--- a/eportal/csv/agric_KG1_result.xlsx
+++ b/eportal/csv/agric_KG1_result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Osotech Software\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\smatechportal\eportal\csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D11884-37A3-48D5-8DAC-0E59E3918605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B411C5-EA1E-4995-B97A-84331CCA1F2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{C92B61B0-82B7-4807-AC1F-A11CBDAD05A6}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C92B61B0-82B7-4807-AC1F-A11CBDAD05A6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -44,7 +36,7 @@
     <t>EXAM SCORE</t>
   </si>
   <si>
-    <t>2021C263130001</t>
+    <t>2021C123450003</t>
   </si>
 </sst>
 </file>
@@ -399,7 +391,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>